<commit_message>
adding oops concept and status colunm
</commit_message>
<xml_diff>
--- a/TS_EMPDET_Project/demo1.xlsx
+++ b/TS_EMPDET_Project/demo1.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
-  <si>
-    <t xml:space="preserve">S.no</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+  <si>
+    <t xml:space="preserve">S.No.</t>
   </si>
   <si>
     <t xml:space="preserve">EmployeeName</t>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bench Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
   </si>
   <si>
     <t xml:space="preserve">Vijay Balakula</t>
@@ -222,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,18 +244,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -287,7 +278,7 @@
   <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -311,22 +302,22 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -338,630 +329,632 @@
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="9"/>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="9" t="n">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6" t="n">
         <v>44409</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="9" t="n">
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="n">
         <v>44448</v>
       </c>
-      <c r="G2" s="9" t="n">
+      <c r="G2" s="6" t="n">
         <v>44491</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="9" t="n">
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="6" t="n">
         <v>44593</v>
       </c>
-      <c r="J2" s="9" t="n">
+      <c r="J2" s="6" t="n">
         <v>44835</v>
       </c>
       <c r="K2" s="0"/>
       <c r="L2" s="3"/>
-      <c r="N2" s="9"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>44410</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="9" t="n">
-        <v>44410</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="6" t="n">
         <v>44464</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>17</v>
+      <c r="G3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="K3" s="0"/>
       <c r="L3" s="3"/>
-      <c r="N3" s="9"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>44411</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="9" t="n">
-        <v>44411</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="9" t="n">
+      <c r="F4" s="6" t="n">
         <v>44469</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>17</v>
+      <c r="G4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="K4" s="0"/>
       <c r="L4" s="3"/>
-      <c r="N4" s="9"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>44412</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="9" t="n">
-        <v>44412</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="6" t="n">
         <v>44461</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="6" t="n">
         <v>44472</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="9" t="n">
+      <c r="H5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="6" t="n">
         <v>44596</v>
       </c>
-      <c r="J5" s="9" t="n">
+      <c r="J5" s="6" t="n">
         <v>44844</v>
       </c>
       <c r="K5" s="0"/>
       <c r="L5" s="3"/>
-      <c r="N5" s="9"/>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>44413</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="9" t="n">
-        <v>44413</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="6" t="n">
         <v>44452</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="6" t="n">
         <v>44479</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="9" t="n">
+      <c r="H6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="6" t="n">
         <v>44603</v>
       </c>
-      <c r="J6" s="9" t="n">
+      <c r="J6" s="6" t="n">
         <v>44839</v>
       </c>
       <c r="K6" s="0"/>
       <c r="L6" s="3"/>
-      <c r="N6" s="9"/>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>44414</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="9" t="n">
-        <v>44414</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="6" t="n">
         <v>44453</v>
       </c>
-      <c r="G7" s="9" t="n">
+      <c r="G7" s="6" t="n">
         <v>44496</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="9" t="n">
+      <c r="H7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="6" t="n">
         <v>44620</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>17</v>
+      <c r="J7" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="K7" s="0"/>
       <c r="L7" s="3"/>
-      <c r="N7" s="9"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="9" t="n">
+        <v>32</v>
+      </c>
+      <c r="D8" s="6" t="n">
         <v>44415</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="9" t="n">
+      <c r="E8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="6" t="n">
         <v>44454</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="9" t="n">
+      <c r="G8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="6" t="n">
         <v>44599</v>
       </c>
-      <c r="J8" s="9" t="n">
+      <c r="J8" s="6" t="n">
         <v>44856</v>
       </c>
       <c r="K8" s="0"/>
       <c r="L8" s="3"/>
-      <c r="N8" s="9"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="D9" s="6" t="n">
         <v>44416</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="9" t="n">
+      <c r="E9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="6" t="n">
         <v>44455</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="9" t="n">
+      <c r="G9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="6" t="n">
         <v>44616</v>
       </c>
-      <c r="J9" s="9" t="n">
+      <c r="J9" s="6" t="n">
         <v>44842</v>
       </c>
       <c r="K9" s="0"/>
       <c r="L9" s="3"/>
-      <c r="N9" s="9"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="9" t="n">
+        <v>36</v>
+      </c>
+      <c r="D10" s="6" t="n">
         <v>44417</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>17</v>
+      <c r="E10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="K10" s="0"/>
       <c r="L10" s="3"/>
-      <c r="N10" s="9"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="K11" s="0"/>
-      <c r="N11" s="9"/>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="K12" s="0"/>
-      <c r="N12" s="9"/>
+      <c r="N12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="K13" s="0"/>
-      <c r="N13" s="9"/>
+      <c r="N13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="K14" s="0"/>
-      <c r="N14" s="9"/>
+      <c r="N14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="K15" s="10"/>
-      <c r="N15" s="9"/>
+      <c r="K15" s="7"/>
+      <c r="N15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="K16" s="0"/>
-      <c r="N16" s="9"/>
+      <c r="N16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="K17" s="0"/>
-      <c r="N17" s="9"/>
+      <c r="N17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="K18" s="0"/>
-      <c r="N18" s="9"/>
+      <c r="N18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="K19" s="0"/>
-      <c r="N19" s="9"/>
+      <c r="N19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="K20" s="0"/>
-      <c r="N20" s="9"/>
+      <c r="N20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="K21" s="0"/>
-      <c r="N21" s="9"/>
+      <c r="N21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="K22" s="0"/>
-      <c r="N22" s="9"/>
+      <c r="N22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="K23" s="0"/>
-      <c r="N23" s="9"/>
+      <c r="N23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="K24" s="0"/>
-      <c r="N24" s="9"/>
+      <c r="N24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="K25" s="0"/>
-      <c r="N25" s="9"/>
+      <c r="N25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="K26" s="0"/>
-      <c r="N26" s="9"/>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="K27" s="0"/>
-      <c r="N27" s="9"/>
+      <c r="N27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="K28" s="0"/>
-      <c r="N28" s="9"/>
+      <c r="N28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="K29" s="0"/>
-      <c r="N29" s="9"/>
+      <c r="N29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="K30" s="0"/>
-      <c r="N30" s="9"/>
+      <c r="N30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="K31" s="0"/>
-      <c r="N31" s="9"/>
+      <c r="N31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="K32" s="0"/>
-      <c r="N32" s="9"/>
+      <c r="N32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="K33" s="0"/>
-      <c r="N33" s="9"/>
+      <c r="N33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="K34" s="0"/>
-      <c r="N34" s="9"/>
+      <c r="N34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="K35" s="0"/>
-      <c r="N35" s="9"/>
+      <c r="N35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="K36" s="0"/>
-      <c r="N36" s="9"/>
+      <c r="N36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="K37" s="0"/>
-      <c r="N37" s="9"/>
+      <c r="N37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="K38" s="0"/>
-      <c r="N38" s="9"/>
+      <c r="N38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="K39" s="0"/>
-      <c r="N39" s="9"/>
+      <c r="N39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="K40" s="0"/>
-      <c r="N40" s="9"/>
+      <c r="N40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="N41" s="9"/>
+      <c r="N41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="N42" s="9"/>
+      <c r="N42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="N43" s="9"/>
+      <c r="N43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="N44" s="9"/>
+      <c r="N44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="N45" s="9"/>
+      <c r="N45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="N46" s="9"/>
+      <c r="N46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N47" s="9"/>
+      <c r="N47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N48" s="9"/>
+      <c r="N48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N49" s="9"/>
+      <c r="N49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N50" s="9"/>
+      <c r="N50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N51" s="9"/>
+      <c r="N51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N52" s="9"/>
+      <c r="N52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N53" s="9"/>
+      <c r="N53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N54" s="9"/>
+      <c r="N54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N55" s="9"/>
+      <c r="N55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N56" s="9"/>
+      <c r="N56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N57" s="9"/>
+      <c r="N57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N58" s="9"/>
+      <c r="N58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N59" s="9"/>
+      <c r="N59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N60" s="9"/>
+      <c r="N60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N61" s="9"/>
+      <c r="N61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N62" s="9"/>
+      <c r="N62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N63" s="9"/>
+      <c r="N63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N64" s="9"/>
+      <c r="N64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N65" s="9"/>
+      <c r="N65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N66" s="9"/>
+      <c r="N66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N67" s="9"/>
+      <c r="N67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N68" s="9"/>
+      <c r="N68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N69" s="9"/>
+      <c r="N69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N70" s="9"/>
+      <c r="N70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N71" s="9"/>
+      <c r="N71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N72" s="9"/>
+      <c r="N72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N73" s="9"/>
+      <c r="N73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N74" s="9"/>
+      <c r="N74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N75" s="9"/>
+      <c r="N75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N76" s="9"/>
+      <c r="N76" s="6"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N77" s="9"/>
+      <c r="N77" s="6"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N78" s="9"/>
+      <c r="N78" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>